<commit_message>
Finished implementing SNS API, including error handling and all planned supported functions
</commit_message>
<xml_diff>
--- a/source/_docs/Error Codes - AWS Toolkit - SNS.xlsx
+++ b/source/_docs/Error Codes - AWS Toolkit - SNS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Code</t>
   </si>
@@ -42,6 +42,18 @@
   </si>
   <si>
     <t>TopicLimitExceeded - The user already owns the maximum allowed number of topics.</t>
+  </si>
+  <si>
+    <t>The 'Set Subscription Attribute' VI only allows setting the 'DeliveryPolicy' and 'RawMessageDelivery' attributes.</t>
+  </si>
+  <si>
+    <t>EndpointDisabled - The specified endpoint is disabled.</t>
+  </si>
+  <si>
+    <t>ParameterValueInvalid - A request parameter does not comply with the associated constraints.</t>
+  </si>
+  <si>
+    <t>PlatformApplicationDisabled - The specified platform application is disabled.</t>
   </si>
 </sst>
 </file>
@@ -420,7 +432,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,6 +481,38 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>412204</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>412205</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>412206</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>412207</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="10" spans="1:2" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>

</xml_diff>

<commit_message>
Updated error codes text files
</commit_message>
<xml_diff>
--- a/source/_docs/Error Codes - AWS Toolkit - SNS.xlsx
+++ b/source/_docs/Error Codes - AWS Toolkit - SNS.xlsx
@@ -97,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -105,15 +105,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -429,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,10 +504,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>